<commit_message>
Minor  Change :: all onboarding version2
</commit_message>
<xml_diff>
--- a/public/assets/ABSQuickOnboarding.xlsx
+++ b/public/assets/ABSQuickOnboarding.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\codings\lara_abs_pms\public\assets\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="125725" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -24,10 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
-  <si>
-    <t xml:space="preserve">Employee Code </t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Employee Name</t>
   </si>
@@ -38,9 +30,6 @@
     <t>DOJ</t>
   </si>
   <si>
-    <t xml:space="preserve">Designation </t>
-  </si>
-  <si>
     <t>L1 Manager Code</t>
   </si>
   <si>
@@ -83,38 +72,29 @@
     <t>EPF Employee</t>
   </si>
   <si>
-    <t xml:space="preserve">ESIC Employee </t>
-  </si>
-  <si>
     <t>Professional Tax</t>
   </si>
   <si>
     <t>Labour Welfare Fund</t>
   </si>
   <si>
-    <t>Emp code</t>
-  </si>
-  <si>
-    <t>Employee</t>
-  </si>
-  <si>
-    <t>test@gmail.com</t>
-  </si>
-  <si>
-    <t>01-01-2000</t>
-  </si>
-  <si>
-    <t>Executive Admin and HR</t>
-  </si>
-  <si>
     <t>Mobile Number</t>
+  </si>
+  <si>
+    <t>Employee Code</t>
+  </si>
+  <si>
+    <t>Designation</t>
+  </si>
+  <si>
+    <t>ESIC Employee</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -126,14 +106,6 @@
       <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0563C1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -177,19 +149,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -316,7 +284,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -351,7 +319,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -528,21 +496,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:W1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.140625" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" customWidth="1"/>
@@ -566,149 +534,78 @@
     <col min="23" max="23" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" s="2" customFormat="1" ht="15.75">
       <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2">
-        <v>9999988888</v>
-      </c>
-      <c r="F2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H2">
-        <v>13205</v>
-      </c>
-      <c r="I2">
-        <v>6603</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>2200</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="P2">
-        <v>1800</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="R2">
-        <v>0</v>
-      </c>
-      <c r="S2">
-        <v>0</v>
-      </c>
-      <c r="T2">
-        <v>1800</v>
-      </c>
-      <c r="U2">
-        <v>0</v>
-      </c>
-      <c r="V2">
-        <v>208</v>
-      </c>
-      <c r="W2">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>

<commit_message>
Minor Change :: Onboarding Version 2 implemeted
</commit_message>
<xml_diff>
--- a/public/assets/ABSQuickOnboarding.xlsx
+++ b/public/assets/ABSQuickOnboarding.xlsx
@@ -496,7 +496,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -507,7 +507,7 @@
   <dimension ref="A1:W1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Minor Change :: Excel data column added
</commit_message>
<xml_diff>
--- a/public/assets/ABSQuickOnboarding.xlsx
+++ b/public/assets/ABSQuickOnboarding.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725" iterateDelta="1E-4"/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Employee Name</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>ESIC Employee</t>
+  </si>
+  <si>
+    <t>Legal Entity</t>
   </si>
 </sst>
 </file>
@@ -496,7 +499,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -504,37 +507,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:W1"/>
+  <dimension ref="A1:X1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.140625" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" customWidth="1"/>
-    <col min="3" max="3" width="23.5703125" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" customWidth="1"/>
-    <col min="7" max="7" width="25.140625" customWidth="1"/>
-    <col min="10" max="10" width="17.7109375" customWidth="1"/>
-    <col min="11" max="11" width="26.28515625" customWidth="1"/>
-    <col min="12" max="12" width="12.28515625" customWidth="1"/>
-    <col min="14" max="14" width="17.42578125" customWidth="1"/>
-    <col min="15" max="15" width="15.5703125" customWidth="1"/>
-    <col min="16" max="16" width="28.7109375" customWidth="1"/>
-    <col min="17" max="17" width="30.85546875" customWidth="1"/>
-    <col min="18" max="18" width="14.28515625" customWidth="1"/>
-    <col min="19" max="19" width="13.42578125" customWidth="1"/>
-    <col min="20" max="20" width="15.42578125" customWidth="1"/>
-    <col min="21" max="21" width="18.28515625" customWidth="1"/>
-    <col min="22" max="22" width="16.28515625" customWidth="1"/>
-    <col min="23" max="23" width="20.7109375" customWidth="1"/>
+    <col min="2" max="3" width="16.28515625" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" customWidth="1"/>
+    <col min="8" max="8" width="25.140625" customWidth="1"/>
+    <col min="11" max="11" width="17.7109375" customWidth="1"/>
+    <col min="12" max="12" width="26.28515625" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" customWidth="1"/>
+    <col min="15" max="15" width="17.42578125" customWidth="1"/>
+    <col min="16" max="16" width="15.5703125" customWidth="1"/>
+    <col min="17" max="17" width="28.7109375" customWidth="1"/>
+    <col min="18" max="18" width="30.85546875" customWidth="1"/>
+    <col min="19" max="19" width="14.28515625" customWidth="1"/>
+    <col min="20" max="20" width="13.42578125" customWidth="1"/>
+    <col min="21" max="21" width="15.42578125" customWidth="1"/>
+    <col min="22" max="22" width="18.28515625" customWidth="1"/>
+    <col min="23" max="23" width="16.28515625" customWidth="1"/>
+    <col min="24" max="24" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="2" customFormat="1" ht="15.75">
+    <row r="1" spans="1:24" s="2" customFormat="1" ht="15.75">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -542,66 +545,69 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Minor Change :: onboarding Excel sheet
</commit_message>
<xml_diff>
--- a/public/assets/ABSQuickOnboarding.xlsx
+++ b/public/assets/ABSQuickOnboarding.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Employee Name</t>
   </si>
@@ -91,6 +91,12 @@
   </si>
   <si>
     <t>Legal Entity</t>
+  </si>
+  <si>
+    <t>Gross</t>
+  </si>
+  <si>
+    <t>CTC</t>
   </si>
 </sst>
 </file>
@@ -499,7 +505,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -507,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:X1"/>
+  <dimension ref="A1:Z1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
@@ -526,18 +532,18 @@
     <col min="12" max="12" width="26.28515625" customWidth="1"/>
     <col min="13" max="13" width="12.28515625" customWidth="1"/>
     <col min="15" max="15" width="17.42578125" customWidth="1"/>
-    <col min="16" max="16" width="15.5703125" customWidth="1"/>
-    <col min="17" max="17" width="28.7109375" customWidth="1"/>
-    <col min="18" max="18" width="30.85546875" customWidth="1"/>
-    <col min="19" max="19" width="14.28515625" customWidth="1"/>
-    <col min="20" max="20" width="13.42578125" customWidth="1"/>
-    <col min="21" max="21" width="15.42578125" customWidth="1"/>
-    <col min="22" max="22" width="18.28515625" customWidth="1"/>
-    <col min="23" max="23" width="16.28515625" customWidth="1"/>
-    <col min="24" max="24" width="20.7109375" customWidth="1"/>
+    <col min="16" max="17" width="15.5703125" customWidth="1"/>
+    <col min="18" max="18" width="28.7109375" customWidth="1"/>
+    <col min="19" max="19" width="30.85546875" customWidth="1"/>
+    <col min="20" max="20" width="14.28515625" customWidth="1"/>
+    <col min="21" max="22" width="13.42578125" customWidth="1"/>
+    <col min="23" max="23" width="15.42578125" customWidth="1"/>
+    <col min="24" max="24" width="18.28515625" customWidth="1"/>
+    <col min="25" max="25" width="16.28515625" customWidth="1"/>
+    <col min="26" max="26" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="2" customFormat="1" ht="15.75">
+    <row r="1" spans="1:26" s="2" customFormat="1" ht="15.75">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -587,27 +593,33 @@
         <v>11</v>
       </c>
       <c r="Q1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="W1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Minor Change :: onboarding ->send appointment letter
</commit_message>
<xml_diff>
--- a/public/assets/ABSQuickOnboarding.xlsx
+++ b/public/assets/ABSQuickOnboarding.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Employee Name</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>CTC</t>
+  </si>
+  <si>
+    <t>Work Location</t>
   </si>
 </sst>
 </file>
@@ -505,7 +508,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -513,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z1"/>
+  <dimension ref="A1:AA1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
+      <selection activeCell="Z15" sqref="Z15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
@@ -526,24 +529,24 @@
     <col min="4" max="4" width="23.5703125" customWidth="1"/>
     <col min="5" max="5" width="14.42578125" customWidth="1"/>
     <col min="6" max="6" width="19.28515625" customWidth="1"/>
-    <col min="7" max="7" width="18.5703125" customWidth="1"/>
-    <col min="8" max="8" width="25.140625" customWidth="1"/>
-    <col min="11" max="11" width="17.7109375" customWidth="1"/>
-    <col min="12" max="12" width="26.28515625" customWidth="1"/>
-    <col min="13" max="13" width="12.28515625" customWidth="1"/>
-    <col min="15" max="15" width="17.42578125" customWidth="1"/>
-    <col min="16" max="17" width="15.5703125" customWidth="1"/>
-    <col min="18" max="18" width="28.7109375" customWidth="1"/>
-    <col min="19" max="19" width="30.85546875" customWidth="1"/>
-    <col min="20" max="20" width="14.28515625" customWidth="1"/>
-    <col min="21" max="22" width="13.42578125" customWidth="1"/>
-    <col min="23" max="23" width="15.42578125" customWidth="1"/>
-    <col min="24" max="24" width="18.28515625" customWidth="1"/>
-    <col min="25" max="25" width="16.28515625" customWidth="1"/>
-    <col min="26" max="26" width="20.7109375" customWidth="1"/>
+    <col min="7" max="8" width="18.5703125" customWidth="1"/>
+    <col min="9" max="9" width="25.140625" customWidth="1"/>
+    <col min="12" max="12" width="17.7109375" customWidth="1"/>
+    <col min="13" max="13" width="26.28515625" customWidth="1"/>
+    <col min="14" max="14" width="12.28515625" customWidth="1"/>
+    <col min="16" max="16" width="17.42578125" customWidth="1"/>
+    <col min="17" max="18" width="15.5703125" customWidth="1"/>
+    <col min="19" max="19" width="28.7109375" customWidth="1"/>
+    <col min="20" max="20" width="30.85546875" customWidth="1"/>
+    <col min="21" max="21" width="14.28515625" customWidth="1"/>
+    <col min="22" max="23" width="13.42578125" customWidth="1"/>
+    <col min="24" max="24" width="15.42578125" customWidth="1"/>
+    <col min="25" max="25" width="18.28515625" customWidth="1"/>
+    <col min="26" max="26" width="16.28515625" customWidth="1"/>
+    <col min="27" max="27" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="2" customFormat="1" ht="15.75">
+    <row r="1" spans="1:27" s="2" customFormat="1" ht="15.75">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -566,60 +569,63 @@
         <v>21</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Minor Change :: onboarding appiontment letter
</commit_message>
<xml_diff>
--- a/public/assets/ABSQuickOnboarding.xlsx
+++ b/public/assets/ABSQuickOnboarding.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Employee Name</t>
   </si>
@@ -100,13 +100,16 @@
   </si>
   <si>
     <t>Work Location</t>
+  </si>
+  <si>
+    <t>Net Income</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -122,8 +125,15 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -134,6 +144,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFF4B183"/>
         <bgColor rgb="FFFF99CC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -164,10 +180,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -508,7 +525,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -516,10 +533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AA1"/>
+  <dimension ref="A1:AB1"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="T1" zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="Z15" sqref="Z15"/>
+      <selection activeCell="X4" sqref="X4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
@@ -539,14 +556,14 @@
     <col min="19" max="19" width="28.7109375" customWidth="1"/>
     <col min="20" max="20" width="30.85546875" customWidth="1"/>
     <col min="21" max="21" width="14.28515625" customWidth="1"/>
-    <col min="22" max="23" width="13.42578125" customWidth="1"/>
-    <col min="24" max="24" width="15.42578125" customWidth="1"/>
-    <col min="25" max="25" width="18.28515625" customWidth="1"/>
-    <col min="26" max="26" width="16.28515625" customWidth="1"/>
-    <col min="27" max="27" width="20.7109375" customWidth="1"/>
+    <col min="22" max="24" width="13.42578125" customWidth="1"/>
+    <col min="25" max="25" width="15.42578125" customWidth="1"/>
+    <col min="26" max="26" width="18.28515625" customWidth="1"/>
+    <col min="27" max="27" width="16.28515625" customWidth="1"/>
+    <col min="28" max="28" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="2" customFormat="1" ht="15.75">
+    <row r="1" spans="1:28" s="2" customFormat="1" ht="15.75">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -616,21 +633,24 @@
       <c r="W1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "Merge branch 'Master' of https://github.com/ABS-Pvt-Ltd/lara_vue_hrms into DockerDeployment"
This reverts commit f65a834fe745b0429475ab99a9a6581afa770ff6, reversing
changes made to 31916b80cc899007b48dcf3a724ca0994906ae55.
</commit_message>
<xml_diff>
--- a/public/assets/ABSQuickOnboarding.xlsx
+++ b/public/assets/ABSQuickOnboarding.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725" iterateDelta="1E-4"/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Employee Name</t>
   </si>
@@ -100,16 +100,13 @@
   </si>
   <si>
     <t>Work Location</t>
-  </si>
-  <si>
-    <t>Net Income</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -125,15 +122,8 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -144,12 +134,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFF4B183"/>
         <bgColor rgb="FFFF99CC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -180,11 +164,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -525,7 +508,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -533,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB1"/>
+  <dimension ref="A1:AA1"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="T1" zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="X4" sqref="X4"/>
+      <selection activeCell="Z15" sqref="Z15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
@@ -556,14 +539,14 @@
     <col min="19" max="19" width="28.7109375" customWidth="1"/>
     <col min="20" max="20" width="30.85546875" customWidth="1"/>
     <col min="21" max="21" width="14.28515625" customWidth="1"/>
-    <col min="22" max="24" width="13.42578125" customWidth="1"/>
-    <col min="25" max="25" width="15.42578125" customWidth="1"/>
-    <col min="26" max="26" width="18.28515625" customWidth="1"/>
-    <col min="27" max="27" width="16.28515625" customWidth="1"/>
-    <col min="28" max="28" width="20.7109375" customWidth="1"/>
+    <col min="22" max="23" width="13.42578125" customWidth="1"/>
+    <col min="24" max="24" width="15.42578125" customWidth="1"/>
+    <col min="25" max="25" width="18.28515625" customWidth="1"/>
+    <col min="26" max="26" width="16.28515625" customWidth="1"/>
+    <col min="27" max="27" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="2" customFormat="1" ht="15.75">
+    <row r="1" spans="1:27" s="2" customFormat="1" ht="15.75">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -633,24 +616,21 @@
       <c r="W1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="X1" s="3" t="s">
-        <v>27</v>
+      <c r="X1" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="AB1" s="1" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Minor Change :: net income column added
</commit_message>
<xml_diff>
--- a/public/assets/ABSQuickOnboarding.xlsx
+++ b/public/assets/ABSQuickOnboarding.xlsx
@@ -525,7 +525,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -535,8 +535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AB1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="X4" sqref="X4"/>
+    <sheetView tabSelected="1" zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>

</xml_diff>